<commit_message>
Update Excel equipment list and re-imported data
</commit_message>
<xml_diff>
--- a/EquipmentList2026.xlsx
+++ b/EquipmentList2026.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JCDC\Desktop\JCDC-main\JCDC-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BDCE22D8-7DF6-442E-AEB6-F78966D85528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{834EAB0C-7F24-4DF1-906C-C65321D48A10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{B941218B-1749-4563-9A81-514A1DFAB1CE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B941218B-1749-4563-9A81-514A1DFAB1CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Supplier Equipment" sheetId="5" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1425" uniqueCount="527">
   <si>
     <t>FLEET CODE</t>
   </si>
@@ -1523,9 +1523,6 @@
     <t>Shantosh Kumar (Lifting Supervisor Day)</t>
   </si>
   <si>
-    <t>Si No</t>
-  </si>
-  <si>
     <t>equipment_name</t>
   </si>
   <si>
@@ -1554,13 +1551,73 @@
   </si>
   <si>
     <t>In Charge Name</t>
+  </si>
+  <si>
+    <t>MAIN LIFT</t>
+  </si>
+  <si>
+    <t>LWJAB200KM07500019</t>
+  </si>
+  <si>
+    <t>SCISSOR LIFT</t>
+  </si>
+  <si>
+    <t>LO30401120</t>
+  </si>
+  <si>
+    <t>LO304978</t>
+  </si>
+  <si>
+    <t>LO3040988</t>
+  </si>
+  <si>
+    <t>LO3040353</t>
+  </si>
+  <si>
+    <t>MD HASSAN</t>
+  </si>
+  <si>
+    <t>SAIDUL ISLAM</t>
+  </si>
+  <si>
+    <t>AKHIYA JAN</t>
+  </si>
+  <si>
+    <t>ABU FARHAN</t>
+  </si>
+  <si>
+    <t>MD DULAL</t>
+  </si>
+  <si>
+    <t>MD ANOWER HOSSEN</t>
+  </si>
+  <si>
+    <t>MD ABDUS SBUR SORKER</t>
+  </si>
+  <si>
+    <t>MD JIBON MIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">General </t>
+  </si>
+  <si>
+    <t>XUG0175ALRRD00258</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AHSAN RAZA IMDAD HUSSAIN </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOHAMMAD FAIZAN JAVED </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trailer </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1600,6 +1657,13 @@
       <name val="Trebuchet MS"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1627,7 +1691,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1650,12 +1714,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1705,12 +1797,64 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 3" xfId="1" xr:uid="{F3517B68-4488-4A8F-BD09-41B7BB3778AD}"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2154,13 +2298,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R153"/>
+  <dimension ref="A1:R165"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="I56" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M1" sqref="M1"/>
+      <selection pane="bottomRight" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2181,49 +2325,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="18" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="15">
+        <v>1</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>497</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>498</v>
       </c>
       <c r="C1" s="15" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="15" t="s">
+        <v>498</v>
+      </c>
+      <c r="E1" s="15" t="s">
         <v>499</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>500</v>
       </c>
       <c r="F1" s="15" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="15" t="s">
+        <v>500</v>
+      </c>
+      <c r="H1" s="15" t="s">
         <v>501</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="I1" s="16" t="s">
         <v>502</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="J1" s="17" t="s">
         <v>503</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="K1" s="15" t="s">
         <v>504</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="L1" s="15" t="s">
         <v>505</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="M1" s="15" t="s">
         <v>506</v>
-      </c>
-      <c r="M1" s="15" t="s">
-        <v>507</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
-        <v>1</v>
+        <f>A1+1</f>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>105</v>
@@ -2264,7 +2409,8 @@
     </row>
     <row r="3" spans="1:13" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
-        <v>1</v>
+        <f t="shared" ref="A3:A66" si="0">A2+1</f>
+        <v>3</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>105</v>
@@ -2305,7 +2451,8 @@
     </row>
     <row r="4" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>105</v>
@@ -2345,8 +2492,9 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A5" s="7">
-        <v>2</v>
+      <c r="A5" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>105</v>
@@ -2386,8 +2534,9 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="7">
-        <v>2</v>
+      <c r="A6" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>105</v>
@@ -2427,8 +2576,9 @@
       </c>
     </row>
     <row r="7" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="7">
-        <v>6</v>
+      <c r="A7" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>105</v>
@@ -2469,7 +2619,8 @@
     </row>
     <row r="8" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
-        <v>7</v>
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>105</v>
@@ -2509,8 +2660,9 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="7">
-        <v>8</v>
+      <c r="A9" s="2">
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>105</v>
@@ -2551,7 +2703,8 @@
     </row>
     <row r="10" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
-        <v>9</v>
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>159</v>
@@ -2574,7 +2727,9 @@
       <c r="H10" s="7">
         <v>2571347232</v>
       </c>
-      <c r="I10" s="7"/>
+      <c r="I10" s="7">
+        <v>1</v>
+      </c>
       <c r="J10" s="5" t="s">
         <v>102</v>
       </c>
@@ -2589,8 +2744,9 @@
       </c>
     </row>
     <row r="11" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A11" s="7">
-        <v>10</v>
+      <c r="A11" s="2">
+        <f t="shared" si="0"/>
+        <v>11</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>159</v>
@@ -2629,7 +2785,8 @@
     </row>
     <row r="12" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>12</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>159</v>
@@ -2669,8 +2826,9 @@
       </c>
     </row>
     <row r="13" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A13" s="7">
-        <v>12</v>
+      <c r="A13" s="2">
+        <f t="shared" si="0"/>
+        <v>13</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>159</v>
@@ -2711,7 +2869,8 @@
     </row>
     <row r="14" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
-        <v>13</v>
+        <f t="shared" si="0"/>
+        <v>14</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>2</v>
@@ -2751,8 +2910,9 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="7">
-        <v>14</v>
+      <c r="A15" s="2">
+        <f t="shared" si="0"/>
+        <v>15</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>2</v>
@@ -2793,7 +2953,8 @@
     </row>
     <row r="16" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
-        <v>15</v>
+        <f t="shared" si="0"/>
+        <v>16</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>90</v>
@@ -2833,8 +2994,9 @@
       </c>
     </row>
     <row r="17" spans="1:13" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A17" s="7">
-        <v>16</v>
+      <c r="A17" s="2">
+        <f t="shared" si="0"/>
+        <v>17</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>90</v>
@@ -2857,7 +3019,9 @@
       <c r="H17" s="7">
         <v>2602039030</v>
       </c>
-      <c r="I17" s="7"/>
+      <c r="I17" s="7">
+        <v>1</v>
+      </c>
       <c r="J17" s="5" t="s">
         <v>95</v>
       </c>
@@ -2873,7 +3037,8 @@
     </row>
     <row r="18" spans="1:13" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
-        <v>17</v>
+        <f t="shared" si="0"/>
+        <v>18</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>59</v>
@@ -2913,8 +3078,9 @@
       </c>
     </row>
     <row r="19" spans="1:13" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A19" s="7">
-        <v>18</v>
+      <c r="A19" s="2">
+        <f t="shared" si="0"/>
+        <v>19</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>59</v>
@@ -2955,7 +3121,8 @@
     </row>
     <row r="20" spans="1:13" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
-        <v>19</v>
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>59</v>
@@ -2995,8 +3162,9 @@
       </c>
     </row>
     <row r="21" spans="1:13" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A21" s="7">
-        <v>20</v>
+      <c r="A21" s="2">
+        <f t="shared" si="0"/>
+        <v>21</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>59</v>
@@ -3037,7 +3205,8 @@
     </row>
     <row r="22" spans="1:13" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
-        <v>21</v>
+        <f t="shared" si="0"/>
+        <v>22</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>73</v>
@@ -3077,8 +3246,9 @@
       </c>
     </row>
     <row r="23" spans="1:13" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A23" s="7">
-        <v>22</v>
+      <c r="A23" s="2">
+        <f t="shared" si="0"/>
+        <v>23</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>27</v>
@@ -3119,7 +3289,8 @@
     </row>
     <row r="24" spans="1:13" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
-        <v>23</v>
+        <f t="shared" si="0"/>
+        <v>24</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>27</v>
@@ -3159,8 +3330,9 @@
       </c>
     </row>
     <row r="25" spans="1:13" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A25" s="7">
-        <v>24</v>
+      <c r="A25" s="2">
+        <f t="shared" si="0"/>
+        <v>25</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>27</v>
@@ -3201,7 +3373,8 @@
     </row>
     <row r="26" spans="1:13" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
-        <v>25</v>
+        <f t="shared" si="0"/>
+        <v>26</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>27</v>
@@ -3241,8 +3414,9 @@
       </c>
     </row>
     <row r="27" spans="1:13" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A27" s="7">
-        <v>26</v>
+      <c r="A27" s="2">
+        <f t="shared" si="0"/>
+        <v>27</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>27</v>
@@ -3283,7 +3457,8 @@
     </row>
     <row r="28" spans="1:13" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
-        <v>27</v>
+        <f t="shared" si="0"/>
+        <v>28</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>27</v>
@@ -3323,8 +3498,9 @@
       </c>
     </row>
     <row r="29" spans="1:13" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A29" s="7">
-        <v>28</v>
+      <c r="A29" s="2">
+        <f t="shared" si="0"/>
+        <v>29</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>27</v>
@@ -3365,7 +3541,8 @@
     </row>
     <row r="30" spans="1:13" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
-        <v>29</v>
+        <f t="shared" si="0"/>
+        <v>30</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>27</v>
@@ -3405,8 +3582,9 @@
       </c>
     </row>
     <row r="31" spans="1:13" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A31" s="7">
-        <v>30</v>
+      <c r="A31" s="2">
+        <f t="shared" si="0"/>
+        <v>31</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>27</v>
@@ -3429,7 +3607,9 @@
       <c r="H31" s="7">
         <v>2613344551</v>
       </c>
-      <c r="I31" s="7"/>
+      <c r="I31" s="7">
+        <v>1</v>
+      </c>
       <c r="J31" s="5" t="s">
         <v>102</v>
       </c>
@@ -3445,7 +3625,8 @@
     </row>
     <row r="32" spans="1:13" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
-        <v>31</v>
+        <f t="shared" si="0"/>
+        <v>32</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>130</v>
@@ -3485,8 +3666,9 @@
       </c>
     </row>
     <row r="33" spans="1:13" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A33" s="7">
-        <v>32</v>
+      <c r="A33" s="2">
+        <f t="shared" si="0"/>
+        <v>33</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>130</v>
@@ -3527,7 +3709,8 @@
     </row>
     <row r="34" spans="1:13" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
-        <v>33</v>
+        <f t="shared" si="0"/>
+        <v>34</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>37</v>
@@ -3567,8 +3750,9 @@
       </c>
     </row>
     <row r="35" spans="1:13" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A35" s="7">
-        <v>34</v>
+      <c r="A35" s="2">
+        <f t="shared" si="0"/>
+        <v>35</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>85</v>
@@ -3609,7 +3793,8 @@
     </row>
     <row r="36" spans="1:13" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
-        <v>35</v>
+        <f t="shared" si="0"/>
+        <v>36</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>19</v>
@@ -3649,8 +3834,9 @@
       </c>
     </row>
     <row r="37" spans="1:13" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A37" s="7">
-        <v>36</v>
+      <c r="A37" s="2">
+        <f t="shared" si="0"/>
+        <v>37</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>19</v>
@@ -3691,7 +3877,8 @@
     </row>
     <row r="38" spans="1:13" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
-        <v>37</v>
+        <f t="shared" si="0"/>
+        <v>38</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>195</v>
@@ -3731,8 +3918,9 @@
       </c>
     </row>
     <row r="39" spans="1:13" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A39" s="7">
-        <v>38</v>
+      <c r="A39" s="2">
+        <f t="shared" si="0"/>
+        <v>39</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>12</v>
@@ -3773,7 +3961,8 @@
     </row>
     <row r="40" spans="1:13" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
-        <v>39</v>
+        <f t="shared" si="0"/>
+        <v>40</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>12</v>
@@ -3811,8 +4000,9 @@
       </c>
     </row>
     <row r="41" spans="1:13" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A41" s="7">
-        <v>40</v>
+      <c r="A41" s="2">
+        <f t="shared" si="0"/>
+        <v>41</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>12</v>
@@ -3853,7 +4043,8 @@
     </row>
     <row r="42" spans="1:13" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
-        <v>41</v>
+        <f t="shared" si="0"/>
+        <v>42</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>12</v>
@@ -3876,7 +4067,9 @@
       <c r="H42" s="7">
         <v>2538148368</v>
       </c>
-      <c r="I42" s="7"/>
+      <c r="I42" s="7">
+        <v>1</v>
+      </c>
       <c r="J42" s="5" t="s">
         <v>102</v>
       </c>
@@ -3891,8 +4084,9 @@
       </c>
     </row>
     <row r="43" spans="1:13" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A43" s="7">
-        <v>42</v>
+      <c r="A43" s="2">
+        <f t="shared" si="0"/>
+        <v>43</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>12</v>
@@ -3915,7 +4109,9 @@
       <c r="H43" s="7">
         <v>2338642248</v>
       </c>
-      <c r="I43" s="7"/>
+      <c r="I43" s="7">
+        <v>1</v>
+      </c>
       <c r="J43" s="5" t="s">
         <v>102</v>
       </c>
@@ -3931,7 +4127,8 @@
     </row>
     <row r="44" spans="1:13" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
-        <v>43</v>
+        <f t="shared" si="0"/>
+        <v>44</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>12</v>
@@ -3971,8 +4168,9 @@
       </c>
     </row>
     <row r="45" spans="1:13" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A45" s="7">
-        <v>44</v>
+      <c r="A45" s="2">
+        <f t="shared" si="0"/>
+        <v>45</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>12</v>
@@ -4013,7 +4211,8 @@
     </row>
     <row r="46" spans="1:13" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
-        <v>45</v>
+        <f t="shared" si="0"/>
+        <v>46</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>12</v>
@@ -4036,7 +4235,9 @@
       <c r="H46" s="7">
         <v>2609856642</v>
       </c>
-      <c r="I46" s="7"/>
+      <c r="I46" s="7">
+        <v>1</v>
+      </c>
       <c r="J46" s="5" t="s">
         <v>17</v>
       </c>
@@ -4051,8 +4252,9 @@
       </c>
     </row>
     <row r="47" spans="1:13" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A47" s="7">
-        <v>46</v>
+      <c r="A47" s="2">
+        <f t="shared" si="0"/>
+        <v>47</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>12</v>
@@ -4093,7 +4295,8 @@
     </row>
     <row r="48" spans="1:13" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
-        <v>47</v>
+        <f t="shared" si="0"/>
+        <v>48</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>12</v>
@@ -4133,8 +4336,9 @@
       </c>
     </row>
     <row r="49" spans="1:13" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A49" s="7">
-        <v>48</v>
+      <c r="A49" s="2">
+        <f t="shared" si="0"/>
+        <v>49</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>12</v>
@@ -4175,7 +4379,8 @@
     </row>
     <row r="50" spans="1:13" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
-        <v>49</v>
+        <f t="shared" si="0"/>
+        <v>50</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>12</v>
@@ -4215,8 +4420,9 @@
       </c>
     </row>
     <row r="51" spans="1:13" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A51" s="7">
-        <v>50</v>
+      <c r="A51" s="2">
+        <f t="shared" si="0"/>
+        <v>51</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>12</v>
@@ -4257,7 +4463,8 @@
     </row>
     <row r="52" spans="1:13" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
-        <v>51</v>
+        <f t="shared" si="0"/>
+        <v>52</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>12</v>
@@ -4293,8 +4500,9 @@
       </c>
     </row>
     <row r="53" spans="1:13" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A53" s="7">
-        <v>52</v>
+      <c r="A53" s="2">
+        <f t="shared" si="0"/>
+        <v>53</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>12</v>
@@ -4333,7 +4541,8 @@
     </row>
     <row r="54" spans="1:13" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
-        <v>53</v>
+        <f t="shared" si="0"/>
+        <v>54</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>12</v>
@@ -4374,7 +4583,8 @@
     </row>
     <row r="55" spans="1:13" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
-        <v>54</v>
+        <f t="shared" si="0"/>
+        <v>55</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>12</v>
@@ -4413,7 +4623,8 @@
     </row>
     <row r="56" spans="1:13" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
-        <v>55</v>
+        <f t="shared" si="0"/>
+        <v>56</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>12</v>
@@ -4452,7 +4663,8 @@
     </row>
     <row r="57" spans="1:13" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>57</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>243</v>
@@ -4491,7 +4703,8 @@
     </row>
     <row r="58" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>58</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>243</v>
@@ -4530,7 +4743,8 @@
     </row>
     <row r="59" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>59</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>243</v>
@@ -4569,7 +4783,8 @@
     </row>
     <row r="60" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>60</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>243</v>
@@ -4608,7 +4823,8 @@
     </row>
     <row r="61" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>61</v>
       </c>
       <c r="B61" s="4" t="s">
         <v>243</v>
@@ -4647,7 +4863,8 @@
     </row>
     <row r="62" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
-        <v>6</v>
+        <f t="shared" si="0"/>
+        <v>62</v>
       </c>
       <c r="B62" s="4" t="s">
         <v>243</v>
@@ -4686,7 +4903,8 @@
     </row>
     <row r="63" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
-        <v>7</v>
+        <f t="shared" si="0"/>
+        <v>63</v>
       </c>
       <c r="B63" s="4" t="s">
         <v>260</v>
@@ -4725,7 +4943,8 @@
     </row>
     <row r="64" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
-        <v>8</v>
+        <f t="shared" si="0"/>
+        <v>64</v>
       </c>
       <c r="B64" s="4" t="s">
         <v>264</v>
@@ -4764,7 +4983,8 @@
     </row>
     <row r="65" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
-        <v>9</v>
+        <f t="shared" si="0"/>
+        <v>65</v>
       </c>
       <c r="B65" s="4" t="s">
         <v>264</v>
@@ -4803,7 +5023,8 @@
     </row>
     <row r="66" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>66</v>
       </c>
       <c r="B66" s="4" t="s">
         <v>264</v>
@@ -4840,7 +5061,8 @@
     </row>
     <row r="67" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
-        <v>11</v>
+        <f t="shared" ref="A67:A130" si="1">A66+1</f>
+        <v>67</v>
       </c>
       <c r="B67" s="4" t="s">
         <v>264</v>
@@ -4879,7 +5101,8 @@
     </row>
     <row r="68" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
-        <v>12</v>
+        <f t="shared" si="1"/>
+        <v>68</v>
       </c>
       <c r="B68" s="4" t="s">
         <v>264</v>
@@ -4918,7 +5141,8 @@
     </row>
     <row r="69" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
-        <v>13</v>
+        <f t="shared" si="1"/>
+        <v>69</v>
       </c>
       <c r="B69" s="4" t="s">
         <v>264</v>
@@ -4957,7 +5181,8 @@
     </row>
     <row r="70" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
-        <v>14</v>
+        <f t="shared" si="1"/>
+        <v>70</v>
       </c>
       <c r="B70" s="4" t="s">
         <v>264</v>
@@ -4996,7 +5221,8 @@
     </row>
     <row r="71" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="2">
-        <v>15</v>
+        <f t="shared" si="1"/>
+        <v>71</v>
       </c>
       <c r="B71" s="4" t="s">
         <v>264</v>
@@ -5035,7 +5261,8 @@
     </row>
     <row r="72" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="2">
-        <v>16</v>
+        <f t="shared" si="1"/>
+        <v>72</v>
       </c>
       <c r="B72" s="4" t="s">
         <v>285</v>
@@ -5074,7 +5301,8 @@
     </row>
     <row r="73" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="2">
-        <v>17</v>
+        <f t="shared" si="1"/>
+        <v>73</v>
       </c>
       <c r="B73" s="4" t="s">
         <v>289</v>
@@ -5113,7 +5341,8 @@
     </row>
     <row r="74" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="2">
-        <v>18</v>
+        <f t="shared" si="1"/>
+        <v>74</v>
       </c>
       <c r="B74" s="4" t="s">
         <v>457</v>
@@ -5152,7 +5381,8 @@
     </row>
     <row r="75" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="2">
-        <v>19</v>
+        <f t="shared" si="1"/>
+        <v>75</v>
       </c>
       <c r="B75" s="4" t="s">
         <v>457</v>
@@ -5191,7 +5421,8 @@
     </row>
     <row r="76" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="2">
-        <v>20</v>
+        <f t="shared" si="1"/>
+        <v>76</v>
       </c>
       <c r="B76" s="4" t="s">
         <v>457</v>
@@ -5230,7 +5461,8 @@
     </row>
     <row r="77" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="2">
-        <v>21</v>
+        <f t="shared" si="1"/>
+        <v>77</v>
       </c>
       <c r="B77" s="4" t="s">
         <v>457</v>
@@ -5269,7 +5501,8 @@
     </row>
     <row r="78" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="2">
-        <v>22</v>
+        <f t="shared" si="1"/>
+        <v>78</v>
       </c>
       <c r="B78" s="4" t="s">
         <v>457</v>
@@ -5308,7 +5541,8 @@
     </row>
     <row r="79" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="2">
-        <v>23</v>
+        <f t="shared" si="1"/>
+        <v>79</v>
       </c>
       <c r="B79" s="4" t="s">
         <v>457</v>
@@ -5347,7 +5581,8 @@
     </row>
     <row r="80" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="2">
-        <v>24</v>
+        <f t="shared" si="1"/>
+        <v>80</v>
       </c>
       <c r="B80" s="4" t="s">
         <v>457</v>
@@ -5363,7 +5598,9 @@
       <c r="G80" s="4" t="s">
         <v>473</v>
       </c>
-      <c r="H80" s="7"/>
+      <c r="H80" s="7">
+        <v>1</v>
+      </c>
       <c r="I80" s="7">
         <v>581782627</v>
       </c>
@@ -5382,7 +5619,8 @@
     </row>
     <row r="81" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="2">
-        <v>25</v>
+        <f t="shared" si="1"/>
+        <v>81</v>
       </c>
       <c r="B81" s="4" t="s">
         <v>457</v>
@@ -5421,7 +5659,8 @@
     </row>
     <row r="82" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="2">
-        <v>26</v>
+        <f t="shared" si="1"/>
+        <v>82</v>
       </c>
       <c r="B82" s="4" t="s">
         <v>457</v>
@@ -5460,7 +5699,8 @@
     </row>
     <row r="83" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="2">
-        <v>27</v>
+        <f t="shared" si="1"/>
+        <v>83</v>
       </c>
       <c r="B83" s="4" t="s">
         <v>457</v>
@@ -5481,7 +5721,9 @@
       <c r="H83" s="7">
         <v>2619027283</v>
       </c>
-      <c r="I83" s="7"/>
+      <c r="I83" s="7">
+        <v>1</v>
+      </c>
       <c r="J83" s="5" t="s">
         <v>246</v>
       </c>
@@ -5497,7 +5739,8 @@
     </row>
     <row r="84" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="2">
-        <v>28</v>
+        <f t="shared" si="1"/>
+        <v>84</v>
       </c>
       <c r="B84" s="4" t="s">
         <v>457</v>
@@ -5536,7 +5779,8 @@
     </row>
     <row r="85" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="2">
-        <v>29</v>
+        <f t="shared" si="1"/>
+        <v>85</v>
       </c>
       <c r="B85" s="4" t="s">
         <v>457</v>
@@ -5575,7 +5819,8 @@
     </row>
     <row r="86" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="2">
-        <v>30</v>
+        <f t="shared" si="1"/>
+        <v>86</v>
       </c>
       <c r="B86" s="4" t="s">
         <v>457</v>
@@ -5596,7 +5841,9 @@
       <c r="H86" s="7">
         <v>2528374557</v>
       </c>
-      <c r="I86" s="7"/>
+      <c r="I86" s="7">
+        <v>1</v>
+      </c>
       <c r="J86" s="5" t="s">
         <v>246</v>
       </c>
@@ -5612,7 +5859,8 @@
     </row>
     <row r="87" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="2">
-        <v>31</v>
+        <f t="shared" si="1"/>
+        <v>87</v>
       </c>
       <c r="B87" s="4" t="s">
         <v>321</v>
@@ -5651,7 +5899,8 @@
     </row>
     <row r="88" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="2">
-        <v>32</v>
+        <f t="shared" si="1"/>
+        <v>88</v>
       </c>
       <c r="B88" s="4" t="s">
         <v>321</v>
@@ -5690,7 +5939,8 @@
     </row>
     <row r="89" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="2">
-        <v>33</v>
+        <f t="shared" si="1"/>
+        <v>89</v>
       </c>
       <c r="B89" s="4" t="s">
         <v>321</v>
@@ -5729,7 +5979,8 @@
     </row>
     <row r="90" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="2">
-        <v>34</v>
+        <f t="shared" si="1"/>
+        <v>90</v>
       </c>
       <c r="B90" s="4" t="s">
         <v>321</v>
@@ -5768,7 +6019,8 @@
     </row>
     <row r="91" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="2">
-        <v>35</v>
+        <f t="shared" si="1"/>
+        <v>91</v>
       </c>
       <c r="B91" s="4" t="s">
         <v>321</v>
@@ -5807,7 +6059,8 @@
     </row>
     <row r="92" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="2">
-        <v>36</v>
+        <f t="shared" si="1"/>
+        <v>92</v>
       </c>
       <c r="B92" s="4" t="s">
         <v>321</v>
@@ -5846,7 +6099,8 @@
     </row>
     <row r="93" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="2">
-        <v>37</v>
+        <f t="shared" si="1"/>
+        <v>93</v>
       </c>
       <c r="B93" s="4" t="s">
         <v>321</v>
@@ -5885,7 +6139,8 @@
     </row>
     <row r="94" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="2">
-        <v>38</v>
+        <f t="shared" si="1"/>
+        <v>94</v>
       </c>
       <c r="B94" s="4" t="s">
         <v>321</v>
@@ -5924,7 +6179,8 @@
     </row>
     <row r="95" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="2">
-        <v>39</v>
+        <f t="shared" si="1"/>
+        <v>95</v>
       </c>
       <c r="B95" s="4" t="s">
         <v>321</v>
@@ -5963,7 +6219,8 @@
     </row>
     <row r="96" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="2">
-        <v>40</v>
+        <f t="shared" si="1"/>
+        <v>96</v>
       </c>
       <c r="B96" s="4" t="s">
         <v>321</v>
@@ -6002,7 +6259,8 @@
     </row>
     <row r="97" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="2">
-        <v>41</v>
+        <f t="shared" si="1"/>
+        <v>97</v>
       </c>
       <c r="B97" s="4" t="s">
         <v>321</v>
@@ -6041,7 +6299,8 @@
     </row>
     <row r="98" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="2">
-        <v>42</v>
+        <f t="shared" si="1"/>
+        <v>98</v>
       </c>
       <c r="B98" s="4" t="s">
         <v>321</v>
@@ -6080,7 +6339,8 @@
     </row>
     <row r="99" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="2">
-        <v>43</v>
+        <f t="shared" si="1"/>
+        <v>99</v>
       </c>
       <c r="B99" s="4" t="s">
         <v>321</v>
@@ -6119,7 +6379,8 @@
     </row>
     <row r="100" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="2">
-        <v>44</v>
+        <f t="shared" si="1"/>
+        <v>100</v>
       </c>
       <c r="B100" s="4" t="s">
         <v>321</v>
@@ -6158,7 +6419,8 @@
     </row>
     <row r="101" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="2">
-        <v>45</v>
+        <f t="shared" si="1"/>
+        <v>101</v>
       </c>
       <c r="B101" s="4" t="s">
         <v>348</v>
@@ -6197,7 +6459,8 @@
     </row>
     <row r="102" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="2">
-        <v>46</v>
+        <f t="shared" si="1"/>
+        <v>102</v>
       </c>
       <c r="B102" s="4" t="s">
         <v>348</v>
@@ -6236,7 +6499,8 @@
     </row>
     <row r="103" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="2">
-        <v>47</v>
+        <f t="shared" si="1"/>
+        <v>103</v>
       </c>
       <c r="B103" s="4" t="s">
         <v>348</v>
@@ -6275,7 +6539,8 @@
     </row>
     <row r="104" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="2">
-        <v>48</v>
+        <f t="shared" si="1"/>
+        <v>104</v>
       </c>
       <c r="B104" s="4" t="s">
         <v>348</v>
@@ -6314,7 +6579,8 @@
     </row>
     <row r="105" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="2">
-        <v>49</v>
+        <f t="shared" si="1"/>
+        <v>105</v>
       </c>
       <c r="B105" s="4" t="s">
         <v>348</v>
@@ -6353,7 +6619,8 @@
     </row>
     <row r="106" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="2">
-        <v>50</v>
+        <f t="shared" si="1"/>
+        <v>106</v>
       </c>
       <c r="B106" s="4" t="s">
         <v>348</v>
@@ -6392,7 +6659,8 @@
     </row>
     <row r="107" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="2">
-        <v>51</v>
+        <f t="shared" si="1"/>
+        <v>107</v>
       </c>
       <c r="B107" s="4" t="s">
         <v>358</v>
@@ -6431,7 +6699,8 @@
     </row>
     <row r="108" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="2">
-        <v>52</v>
+        <f t="shared" si="1"/>
+        <v>108</v>
       </c>
       <c r="B108" s="4" t="s">
         <v>358</v>
@@ -6470,7 +6739,8 @@
     </row>
     <row r="109" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="2">
-        <v>53</v>
+        <f t="shared" si="1"/>
+        <v>109</v>
       </c>
       <c r="B109" s="4" t="s">
         <v>358</v>
@@ -6509,7 +6779,8 @@
     </row>
     <row r="110" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="2">
-        <v>54</v>
+        <f t="shared" si="1"/>
+        <v>110</v>
       </c>
       <c r="B110" s="4" t="s">
         <v>358</v>
@@ -6548,7 +6819,8 @@
     </row>
     <row r="111" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="2">
-        <v>55</v>
+        <f t="shared" si="1"/>
+        <v>111</v>
       </c>
       <c r="B111" s="4" t="s">
         <v>358</v>
@@ -6587,7 +6859,8 @@
     </row>
     <row r="112" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="2">
-        <v>56</v>
+        <f t="shared" si="1"/>
+        <v>112</v>
       </c>
       <c r="B112" s="4" t="s">
         <v>358</v>
@@ -6626,7 +6899,8 @@
     </row>
     <row r="113" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="2">
-        <v>57</v>
+        <f t="shared" si="1"/>
+        <v>113</v>
       </c>
       <c r="B113" s="4" t="s">
         <v>358</v>
@@ -6665,7 +6939,8 @@
     </row>
     <row r="114" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="2">
-        <v>58</v>
+        <f t="shared" si="1"/>
+        <v>114</v>
       </c>
       <c r="B114" s="4" t="s">
         <v>358</v>
@@ -6704,7 +6979,8 @@
     </row>
     <row r="115" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="2">
-        <v>59</v>
+        <f t="shared" si="1"/>
+        <v>115</v>
       </c>
       <c r="B115" s="4" t="s">
         <v>376</v>
@@ -6743,7 +7019,8 @@
     </row>
     <row r="116" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="2">
-        <v>60</v>
+        <f t="shared" si="1"/>
+        <v>116</v>
       </c>
       <c r="B116" s="4" t="s">
         <v>376</v>
@@ -6782,7 +7059,8 @@
     </row>
     <row r="117" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="2">
-        <v>61</v>
+        <f t="shared" si="1"/>
+        <v>117</v>
       </c>
       <c r="B117" s="4" t="s">
         <v>376</v>
@@ -6821,7 +7099,8 @@
     </row>
     <row r="118" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="2">
-        <v>62</v>
+        <f t="shared" si="1"/>
+        <v>118</v>
       </c>
       <c r="B118" s="4" t="s">
         <v>376</v>
@@ -6860,7 +7139,8 @@
     </row>
     <row r="119" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="2">
-        <v>63</v>
+        <f t="shared" si="1"/>
+        <v>119</v>
       </c>
       <c r="B119" s="4" t="s">
         <v>376</v>
@@ -6899,7 +7179,8 @@
     </row>
     <row r="120" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="2">
-        <v>64</v>
+        <f t="shared" si="1"/>
+        <v>120</v>
       </c>
       <c r="B120" s="4" t="s">
         <v>376</v>
@@ -6938,7 +7219,8 @@
     </row>
     <row r="121" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="2">
-        <v>65</v>
+        <f t="shared" si="1"/>
+        <v>121</v>
       </c>
       <c r="B121" s="4" t="s">
         <v>376</v>
@@ -6977,7 +7259,8 @@
     </row>
     <row r="122" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="2">
-        <v>66</v>
+        <f t="shared" si="1"/>
+        <v>122</v>
       </c>
       <c r="B122" s="4" t="s">
         <v>376</v>
@@ -7016,7 +7299,8 @@
     </row>
     <row r="123" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="2">
-        <v>67</v>
+        <f t="shared" si="1"/>
+        <v>123</v>
       </c>
       <c r="B123" s="4" t="s">
         <v>376</v>
@@ -7055,7 +7339,8 @@
     </row>
     <row r="124" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="2">
-        <v>68</v>
+        <f t="shared" si="1"/>
+        <v>124</v>
       </c>
       <c r="B124" s="4" t="s">
         <v>376</v>
@@ -7094,7 +7379,8 @@
     </row>
     <row r="125" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="2">
-        <v>69</v>
+        <f t="shared" si="1"/>
+        <v>125</v>
       </c>
       <c r="B125" s="4" t="s">
         <v>376</v>
@@ -7133,7 +7419,8 @@
     </row>
     <row r="126" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="2">
-        <v>70</v>
+        <f t="shared" si="1"/>
+        <v>126</v>
       </c>
       <c r="B126" s="4" t="s">
         <v>376</v>
@@ -7172,7 +7459,8 @@
     </row>
     <row r="127" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="2">
-        <v>71</v>
+        <f t="shared" si="1"/>
+        <v>127</v>
       </c>
       <c r="B127" s="4" t="s">
         <v>376</v>
@@ -7211,7 +7499,8 @@
     </row>
     <row r="128" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="2">
-        <v>72</v>
+        <f t="shared" si="1"/>
+        <v>128</v>
       </c>
       <c r="B128" s="4" t="s">
         <v>376</v>
@@ -7250,7 +7539,8 @@
     </row>
     <row r="129" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="2">
-        <v>73</v>
+        <f t="shared" si="1"/>
+        <v>129</v>
       </c>
       <c r="B129" s="4" t="s">
         <v>12</v>
@@ -7289,7 +7579,8 @@
     </row>
     <row r="130" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="2">
-        <v>74</v>
+        <f t="shared" si="1"/>
+        <v>130</v>
       </c>
       <c r="B130" s="4" t="s">
         <v>12</v>
@@ -7328,7 +7619,8 @@
     </row>
     <row r="131" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="2">
-        <v>75</v>
+        <f t="shared" ref="A131:A159" si="2">A130+1</f>
+        <v>131</v>
       </c>
       <c r="B131" s="4" t="s">
         <v>406</v>
@@ -7367,7 +7659,8 @@
     </row>
     <row r="132" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="2">
-        <v>76</v>
+        <f t="shared" si="2"/>
+        <v>132</v>
       </c>
       <c r="B132" s="4" t="s">
         <v>406</v>
@@ -7406,7 +7699,8 @@
     </row>
     <row r="133" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="2">
-        <v>77</v>
+        <f t="shared" si="2"/>
+        <v>133</v>
       </c>
       <c r="B133" s="4" t="s">
         <v>406</v>
@@ -7445,7 +7739,8 @@
     </row>
     <row r="134" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="2">
-        <v>78</v>
+        <f t="shared" si="2"/>
+        <v>134</v>
       </c>
       <c r="B134" s="4" t="s">
         <v>406</v>
@@ -7484,7 +7779,8 @@
     </row>
     <row r="135" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="2">
-        <v>79</v>
+        <f t="shared" si="2"/>
+        <v>135</v>
       </c>
       <c r="B135" s="4" t="s">
         <v>406</v>
@@ -7523,7 +7819,8 @@
     </row>
     <row r="136" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="2">
-        <v>80</v>
+        <f t="shared" si="2"/>
+        <v>136</v>
       </c>
       <c r="B136" s="4" t="s">
         <v>406</v>
@@ -7562,7 +7859,8 @@
     </row>
     <row r="137" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="2">
-        <v>81</v>
+        <f t="shared" si="2"/>
+        <v>137</v>
       </c>
       <c r="B137" s="4" t="s">
         <v>406</v>
@@ -7601,7 +7899,8 @@
     </row>
     <row r="138" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="2">
-        <v>82</v>
+        <f t="shared" si="2"/>
+        <v>138</v>
       </c>
       <c r="B138" s="4" t="s">
         <v>406</v>
@@ -7640,7 +7939,8 @@
     </row>
     <row r="139" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" s="2">
-        <v>83</v>
+        <f t="shared" si="2"/>
+        <v>139</v>
       </c>
       <c r="B139" s="4" t="s">
         <v>406</v>
@@ -7679,7 +7979,8 @@
     </row>
     <row r="140" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="2">
-        <v>84</v>
+        <f t="shared" si="2"/>
+        <v>140</v>
       </c>
       <c r="B140" s="4" t="s">
         <v>406</v>
@@ -7718,7 +8019,8 @@
     </row>
     <row r="141" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" s="2">
-        <v>85</v>
+        <f t="shared" si="2"/>
+        <v>141</v>
       </c>
       <c r="B141" s="4" t="s">
         <v>406</v>
@@ -7757,7 +8059,8 @@
     </row>
     <row r="142" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" s="2">
-        <v>86</v>
+        <f t="shared" si="2"/>
+        <v>142</v>
       </c>
       <c r="B142" s="4" t="s">
         <v>428</v>
@@ -7796,7 +8099,8 @@
     </row>
     <row r="143" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="2">
-        <v>87</v>
+        <f t="shared" si="2"/>
+        <v>143</v>
       </c>
       <c r="B143" s="4" t="s">
         <v>428</v>
@@ -7835,7 +8139,8 @@
     </row>
     <row r="144" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="2">
-        <v>88</v>
+        <f t="shared" si="2"/>
+        <v>144</v>
       </c>
       <c r="B144" s="4" t="s">
         <v>432</v>
@@ -7854,7 +8159,9 @@
       <c r="H144" s="7">
         <v>2371258480</v>
       </c>
-      <c r="I144" s="7"/>
+      <c r="I144" s="7">
+        <v>1</v>
+      </c>
       <c r="J144" s="5" t="s">
         <v>246</v>
       </c>
@@ -7870,7 +8177,8 @@
     </row>
     <row r="145" spans="1:18" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="2">
-        <v>89</v>
+        <f t="shared" si="2"/>
+        <v>145</v>
       </c>
       <c r="B145" s="4" t="s">
         <v>432</v>
@@ -7889,7 +8197,9 @@
       <c r="H145" s="7">
         <v>2545277937</v>
       </c>
-      <c r="I145" s="7"/>
+      <c r="I145" s="7">
+        <v>1</v>
+      </c>
       <c r="J145" s="5" t="s">
         <v>246</v>
       </c>
@@ -7905,7 +8215,8 @@
     </row>
     <row r="146" spans="1:18" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="2">
-        <v>90</v>
+        <f t="shared" si="2"/>
+        <v>146</v>
       </c>
       <c r="B146" s="4" t="s">
         <v>432</v>
@@ -7924,7 +8235,9 @@
       <c r="H146" s="7">
         <v>2510755784</v>
       </c>
-      <c r="I146" s="7"/>
+      <c r="I146" s="7">
+        <v>1</v>
+      </c>
       <c r="J146" s="5" t="s">
         <v>246</v>
       </c>
@@ -7940,7 +8253,8 @@
     </row>
     <row r="147" spans="1:18" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="2">
-        <v>91</v>
+        <f t="shared" si="2"/>
+        <v>147</v>
       </c>
       <c r="B147" s="4" t="s">
         <v>432</v>
@@ -7959,7 +8273,9 @@
       <c r="H147" s="7">
         <v>2402689315</v>
       </c>
-      <c r="I147" s="7"/>
+      <c r="I147" s="7">
+        <v>1</v>
+      </c>
       <c r="J147" s="5" t="s">
         <v>246</v>
       </c>
@@ -7975,7 +8291,8 @@
     </row>
     <row r="148" spans="1:18" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" s="2">
-        <v>92</v>
+        <f t="shared" si="2"/>
+        <v>148</v>
       </c>
       <c r="B148" s="4" t="s">
         <v>432</v>
@@ -7994,7 +8311,9 @@
       <c r="H148" s="7">
         <v>2602788081</v>
       </c>
-      <c r="I148" s="7"/>
+      <c r="I148" s="7">
+        <v>1</v>
+      </c>
       <c r="J148" s="5" t="s">
         <v>246</v>
       </c>
@@ -8010,7 +8329,8 @@
     </row>
     <row r="149" spans="1:18" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" s="2">
-        <v>93</v>
+        <f t="shared" si="2"/>
+        <v>149</v>
       </c>
       <c r="B149" s="4" t="s">
         <v>432</v>
@@ -8029,7 +8349,9 @@
       <c r="H149" s="7">
         <v>2293294985</v>
       </c>
-      <c r="I149" s="7"/>
+      <c r="I149" s="7">
+        <v>1</v>
+      </c>
       <c r="J149" s="5" t="s">
         <v>246</v>
       </c>
@@ -8043,33 +8365,523 @@
         <v>495</v>
       </c>
     </row>
-    <row r="150" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A150" s="2">
+        <f t="shared" si="2"/>
+        <v>150</v>
+      </c>
+      <c r="B150" s="19" t="s">
+        <v>507</v>
+      </c>
+      <c r="C150" s="4"/>
+      <c r="D150" s="19">
+        <v>503001447</v>
+      </c>
+      <c r="E150" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F150" s="11">
+        <v>45669</v>
+      </c>
+      <c r="G150" s="20" t="s">
+        <v>514</v>
+      </c>
+      <c r="H150" s="22">
+        <v>2619033927</v>
+      </c>
+      <c r="I150" s="21">
+        <v>552218662</v>
+      </c>
+      <c r="J150" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="K150" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="L150" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="M150" s="1" t="s">
+        <v>522</v>
+      </c>
       <c r="N150" s="6"/>
       <c r="O150" s="6"/>
       <c r="P150" s="6"/>
       <c r="Q150" s="6"/>
       <c r="R150" s="6"/>
     </row>
-    <row r="151" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A151" s="2">
+        <f t="shared" si="2"/>
+        <v>151</v>
+      </c>
+      <c r="B151" s="19" t="s">
+        <v>507</v>
+      </c>
+      <c r="C151" s="4"/>
+      <c r="D151" s="19">
+        <v>503001447</v>
+      </c>
+      <c r="E151" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F151" s="11">
+        <v>45670</v>
+      </c>
+      <c r="G151" s="20" t="s">
+        <v>515</v>
+      </c>
+      <c r="H151" s="22">
+        <v>2619034537</v>
+      </c>
+      <c r="I151" s="21">
+        <v>581669127</v>
+      </c>
+      <c r="J151" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="K151" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="L151" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="M151" s="1" t="s">
+        <v>522</v>
+      </c>
       <c r="N151" s="6"/>
       <c r="O151" s="6"/>
       <c r="P151" s="6"/>
       <c r="Q151" s="6"/>
       <c r="R151" s="6"/>
     </row>
-    <row r="152" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A152" s="2">
+        <f t="shared" si="2"/>
+        <v>152</v>
+      </c>
+      <c r="B152" s="19" t="s">
+        <v>507</v>
+      </c>
+      <c r="C152" s="4"/>
+      <c r="D152" s="19">
+        <v>503001383</v>
+      </c>
+      <c r="E152" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F152" s="11">
+        <v>45671</v>
+      </c>
+      <c r="G152" s="20" t="s">
+        <v>516</v>
+      </c>
+      <c r="H152" s="22">
+        <v>2529002384</v>
+      </c>
+      <c r="I152" s="21">
+        <v>558533083</v>
+      </c>
+      <c r="J152" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="K152" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="L152" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="M152" s="1" t="s">
+        <v>522</v>
+      </c>
       <c r="N152" s="6"/>
       <c r="O152" s="6"/>
       <c r="P152" s="6"/>
       <c r="Q152" s="6"/>
       <c r="R152" s="6"/>
     </row>
-    <row r="153" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A153" s="2">
+        <f t="shared" si="2"/>
+        <v>153</v>
+      </c>
+      <c r="B153" s="19" t="s">
+        <v>507</v>
+      </c>
+      <c r="C153" s="4"/>
+      <c r="D153" s="19" t="s">
+        <v>508</v>
+      </c>
+      <c r="E153" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F153" s="11">
+        <v>45672</v>
+      </c>
+      <c r="G153" s="20" t="s">
+        <v>517</v>
+      </c>
+      <c r="H153" s="22">
+        <v>2619027200</v>
+      </c>
+      <c r="I153" s="21">
+        <v>572385247</v>
+      </c>
+      <c r="J153" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="K153" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="L153" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="M153" s="1" t="s">
+        <v>522</v>
+      </c>
       <c r="N153" s="6"/>
       <c r="O153" s="6"/>
       <c r="P153" s="6"/>
       <c r="Q153" s="6"/>
       <c r="R153" s="6"/>
+    </row>
+    <row r="154" spans="1:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A154" s="2">
+        <f t="shared" si="2"/>
+        <v>154</v>
+      </c>
+      <c r="B154" s="19" t="s">
+        <v>509</v>
+      </c>
+      <c r="C154" s="4"/>
+      <c r="D154" s="19" t="s">
+        <v>510</v>
+      </c>
+      <c r="E154" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F154" s="11">
+        <v>45673</v>
+      </c>
+      <c r="G154" s="20" t="s">
+        <v>518</v>
+      </c>
+      <c r="H154" s="22">
+        <v>2619097583</v>
+      </c>
+      <c r="I154" s="21">
+        <v>563245681</v>
+      </c>
+      <c r="J154" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="K154" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="L154" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="M154" s="1" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="155" spans="1:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A155" s="2">
+        <f t="shared" si="2"/>
+        <v>155</v>
+      </c>
+      <c r="B155" s="19" t="s">
+        <v>509</v>
+      </c>
+      <c r="C155" s="4"/>
+      <c r="D155" s="19" t="s">
+        <v>511</v>
+      </c>
+      <c r="E155" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F155" s="11">
+        <v>45674</v>
+      </c>
+      <c r="G155" s="20" t="s">
+        <v>519</v>
+      </c>
+      <c r="H155" s="22">
+        <v>2621447321</v>
+      </c>
+      <c r="I155" s="21">
+        <v>531682160</v>
+      </c>
+      <c r="J155" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="K155" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="L155" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="M155" s="1" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="156" spans="1:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A156" s="2">
+        <f t="shared" si="2"/>
+        <v>156</v>
+      </c>
+      <c r="B156" s="19" t="s">
+        <v>509</v>
+      </c>
+      <c r="C156" s="4"/>
+      <c r="D156" s="19" t="s">
+        <v>512</v>
+      </c>
+      <c r="E156" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F156" s="11">
+        <v>45675</v>
+      </c>
+      <c r="G156" s="20" t="s">
+        <v>520</v>
+      </c>
+      <c r="H156" s="22">
+        <v>2621465323</v>
+      </c>
+      <c r="I156" s="21">
+        <v>550925696</v>
+      </c>
+      <c r="J156" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="K156" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="L156" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="M156" s="1" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="157" spans="1:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A157" s="2">
+        <f t="shared" si="2"/>
+        <v>157</v>
+      </c>
+      <c r="B157" s="19" t="s">
+        <v>509</v>
+      </c>
+      <c r="C157" s="4"/>
+      <c r="D157" s="19" t="s">
+        <v>513</v>
+      </c>
+      <c r="E157" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F157" s="11">
+        <v>45676</v>
+      </c>
+      <c r="G157" s="20" t="s">
+        <v>521</v>
+      </c>
+      <c r="H157" s="22">
+        <v>2619028604</v>
+      </c>
+      <c r="I157" s="21">
+        <v>552113039</v>
+      </c>
+      <c r="J157" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="K157" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="L157" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="M157" s="1" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="158" spans="1:18" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A158" s="2">
+        <f t="shared" si="2"/>
+        <v>158</v>
+      </c>
+      <c r="B158" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="C158" s="4"/>
+      <c r="D158" s="4" t="s">
+        <v>523</v>
+      </c>
+      <c r="E158" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F158" s="11">
+        <v>45677</v>
+      </c>
+      <c r="G158" s="4" t="s">
+        <v>524</v>
+      </c>
+      <c r="H158" s="7">
+        <v>2550483701</v>
+      </c>
+      <c r="I158" s="7">
+        <v>502179038</v>
+      </c>
+      <c r="J158" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="K158" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="L158" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="M158" s="1" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="159" spans="1:18" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A159" s="2">
+        <f t="shared" si="2"/>
+        <v>159</v>
+      </c>
+      <c r="B159" s="4" t="s">
+        <v>526</v>
+      </c>
+      <c r="C159" s="4"/>
+      <c r="D159" s="4"/>
+      <c r="E159" s="4"/>
+      <c r="F159" s="11">
+        <v>45678</v>
+      </c>
+      <c r="G159" s="4" t="s">
+        <v>525</v>
+      </c>
+      <c r="H159" s="7">
+        <v>2622079818</v>
+      </c>
+      <c r="I159" s="7">
+        <v>573380318</v>
+      </c>
+      <c r="J159" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="K159" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="L159" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="M159" s="1" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="160" spans="1:18" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A160" s="2"/>
+      <c r="B160" s="4"/>
+      <c r="C160" s="4"/>
+      <c r="D160" s="4"/>
+      <c r="E160" s="4"/>
+      <c r="F160" s="11">
+        <v>45679</v>
+      </c>
+      <c r="G160" s="4"/>
+      <c r="H160" s="7"/>
+      <c r="I160" s="7"/>
+      <c r="J160" s="5"/>
+      <c r="K160" s="14"/>
+      <c r="L160" s="4"/>
+      <c r="M160" s="1"/>
+    </row>
+    <row r="161" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A161" s="2"/>
+      <c r="B161" s="4"/>
+      <c r="C161" s="4"/>
+      <c r="D161" s="4"/>
+      <c r="E161" s="4"/>
+      <c r="F161" s="11">
+        <v>45680</v>
+      </c>
+      <c r="G161" s="4"/>
+      <c r="H161" s="7"/>
+      <c r="I161" s="7"/>
+      <c r="J161" s="5"/>
+      <c r="K161" s="14"/>
+      <c r="L161" s="4"/>
+      <c r="M161" s="1"/>
+    </row>
+    <row r="162" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A162" s="2"/>
+      <c r="B162" s="4"/>
+      <c r="C162" s="4"/>
+      <c r="D162" s="4"/>
+      <c r="E162" s="4"/>
+      <c r="F162" s="11">
+        <v>45681</v>
+      </c>
+      <c r="G162" s="4"/>
+      <c r="H162" s="7"/>
+      <c r="I162" s="7"/>
+      <c r="J162" s="5"/>
+      <c r="K162" s="14"/>
+      <c r="L162" s="4"/>
+      <c r="M162" s="1"/>
+    </row>
+    <row r="163" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A163" s="2"/>
+      <c r="B163" s="4"/>
+      <c r="C163" s="4"/>
+      <c r="D163" s="4"/>
+      <c r="E163" s="4"/>
+      <c r="F163" s="11">
+        <v>45682</v>
+      </c>
+      <c r="G163" s="4"/>
+      <c r="H163" s="7"/>
+      <c r="I163" s="7"/>
+      <c r="J163" s="5"/>
+      <c r="K163" s="14"/>
+      <c r="L163" s="4"/>
+      <c r="M163" s="1"/>
+    </row>
+    <row r="164" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A164" s="2"/>
+      <c r="B164" s="4"/>
+      <c r="C164" s="4"/>
+      <c r="D164" s="4"/>
+      <c r="E164" s="4"/>
+      <c r="F164" s="11">
+        <v>45683</v>
+      </c>
+      <c r="G164" s="4"/>
+      <c r="H164" s="7"/>
+      <c r="I164" s="7"/>
+      <c r="J164" s="5"/>
+      <c r="K164" s="14"/>
+      <c r="L164" s="4"/>
+      <c r="M164" s="1"/>
+    </row>
+    <row r="165" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A165" s="2"/>
+      <c r="B165" s="4"/>
+      <c r="C165" s="4"/>
+      <c r="D165" s="4"/>
+      <c r="E165" s="4"/>
+      <c r="F165" s="11">
+        <v>45684</v>
+      </c>
+      <c r="G165" s="4"/>
+      <c r="H165" s="7"/>
+      <c r="I165" s="7"/>
+      <c r="J165" s="5"/>
+      <c r="K165" s="14"/>
+      <c r="L165" s="4"/>
+      <c r="M165" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:M149" xr:uid="{9AEAC16E-221F-49E8-9C2A-7CA8F46B2CE6}">
@@ -8078,38 +8890,44 @@
     </sortState>
   </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="G1:G2 G4:G1048576">
-    <cfRule type="duplicateValues" dxfId="10" priority="201"/>
+  <conditionalFormatting sqref="G1:G2 G4:G149 G158:G1048576">
+    <cfRule type="duplicateValues" dxfId="14" priority="205"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G44:G56">
-    <cfRule type="duplicateValues" dxfId="9" priority="219"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="223"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G57:G149">
-    <cfRule type="duplicateValues" dxfId="8" priority="396"/>
+  <conditionalFormatting sqref="G57:G149 G158:G165">
+    <cfRule type="duplicateValues" dxfId="12" priority="400"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G150:G1048576 G1:G2 G4:G43">
-    <cfRule type="duplicateValues" dxfId="7" priority="205"/>
+  <conditionalFormatting sqref="G166:G1048576 G1:G2 G4:G43">
+    <cfRule type="duplicateValues" dxfId="11" priority="209"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="duplicateValues" dxfId="6" priority="191"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="195"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17:H20">
-    <cfRule type="duplicateValues" dxfId="5" priority="212"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="216"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21:H24">
-    <cfRule type="duplicateValues" dxfId="4" priority="210"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="214"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25">
-    <cfRule type="duplicateValues" dxfId="3" priority="209"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="213"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26:H43">
-    <cfRule type="duplicateValues" dxfId="2" priority="208"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="212"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H44:H56">
-    <cfRule type="duplicateValues" dxfId="1" priority="217"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="221"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H57:H149">
-    <cfRule type="duplicateValues" dxfId="0" priority="398"/>
+  <conditionalFormatting sqref="H57:H149 H158:H165">
+    <cfRule type="duplicateValues" dxfId="4" priority="402"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D150:D156">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I150:I157">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="39" fitToHeight="0" orientation="landscape" verticalDpi="0" r:id="rId1"/>

</xml_diff>